<commit_message>
add a few files
</commit_message>
<xml_diff>
--- a/Models_Information.xlsx
+++ b/Models_Information.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\onnx\tflite2semantic\tinyML\collected_models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\tinyml-research-symposium-2022-haoyu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4266953D-5160-4C8D-B4A5-A1E4E3389B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F390B0-8FC3-47AF-8BC9-77D3A4A38E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -291,9 +291,6 @@
     <t>0: right, 1: left</t>
   </si>
   <si>
-    <t>tested on MP34DT05</t>
-  </si>
-  <si>
     <t>tested on OV7675/0</t>
   </si>
   <si>
@@ -364,6 +361,9 @@
   </si>
   <si>
     <t>https://github.com/Haoyu-R/TinyML-Research-Symposium-2022/tree/main/model_repo</t>
+  </si>
+  <si>
+    <t>tested on MP34DT05 20000 sps</t>
   </si>
 </sst>
 </file>
@@ -706,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -780,10 +780,10 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
@@ -798,22 +798,22 @@
         <v>3</v>
       </c>
       <c r="I2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K2" t="s">
         <v>16</v>
       </c>
       <c r="L2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M2" t="s">
         <v>17</v>
       </c>
       <c r="N2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
@@ -842,22 +842,22 @@
         <v>4</v>
       </c>
       <c r="I3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K3" t="s">
         <v>22</v>
       </c>
       <c r="L3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M3" t="s">
         <v>23</v>
       </c>
       <c r="N3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
@@ -868,13 +868,13 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -886,7 +886,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J4" t="s">
         <v>32</v>
@@ -895,13 +895,13 @@
         <v>33</v>
       </c>
       <c r="L4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M4" t="s">
         <v>23</v>
       </c>
       <c r="N4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
@@ -912,7 +912,7 @@
         <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D5" t="s">
         <v>42</v>
@@ -930,7 +930,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J5" t="s">
         <v>39</v>
@@ -939,13 +939,13 @@
         <v>40</v>
       </c>
       <c r="L5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M5" t="s">
         <v>35</v>
       </c>
       <c r="N5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
@@ -956,7 +956,7 @@
         <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D6" t="s">
         <v>55</v>
@@ -974,22 +974,22 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K6" t="s">
         <v>41</v>
       </c>
       <c r="L6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M6" t="s">
         <v>44</v>
       </c>
       <c r="N6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -1000,7 +1000,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="D7" t="s">
         <v>67</v>
@@ -1018,7 +1018,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J7" t="s">
         <v>53</v>
@@ -1027,13 +1027,13 @@
         <v>18</v>
       </c>
       <c r="L7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M7" t="s">
         <v>17</v>
       </c>
       <c r="N7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
@@ -1044,7 +1044,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="D8" t="s">
         <v>67</v>
@@ -1062,7 +1062,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J8" t="s">
         <v>53</v>
@@ -1071,13 +1071,13 @@
         <v>45</v>
       </c>
       <c r="L8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M8" t="s">
         <v>35</v>
       </c>
       <c r="N8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -1088,7 +1088,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="D9" t="s">
         <v>67</v>
@@ -1106,7 +1106,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J9" t="s">
         <v>53</v>
@@ -1115,13 +1115,13 @@
         <v>46</v>
       </c>
       <c r="L9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M9" t="s">
         <v>23</v>
       </c>
       <c r="N9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -1132,7 +1132,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="D10" t="s">
         <v>67</v>
@@ -1150,7 +1150,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J10" t="s">
         <v>53</v>
@@ -1159,13 +1159,13 @@
         <v>46</v>
       </c>
       <c r="L10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M10" t="s">
         <v>17</v>
       </c>
       <c r="N10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -1176,7 +1176,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="D11" t="s">
         <v>67</v>
@@ -1194,7 +1194,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J11" t="s">
         <v>53</v>
@@ -1203,13 +1203,13 @@
         <v>46</v>
       </c>
       <c r="L11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M11" t="s">
         <v>17</v>
       </c>
       <c r="N11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
@@ -1220,7 +1220,7 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="D12" t="s">
         <v>67</v>
@@ -1238,7 +1238,7 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J12" t="s">
         <v>53</v>
@@ -1247,13 +1247,13 @@
         <v>46</v>
       </c>
       <c r="L12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M12" t="s">
         <v>17</v>
       </c>
       <c r="N12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
@@ -1264,7 +1264,7 @@
         <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D13" t="s">
         <v>81</v>
@@ -1282,22 +1282,22 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J13" t="s">
         <v>69</v>
       </c>
       <c r="K13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M13" t="s">
         <v>17</v>
       </c>
       <c r="N13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
@@ -1308,7 +1308,7 @@
         <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D14" t="s">
         <v>81</v>
@@ -1326,22 +1326,22 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J14" t="s">
         <v>69</v>
       </c>
       <c r="K14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M14" t="s">
         <v>17</v>
       </c>
       <c r="N14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
@@ -1352,7 +1352,7 @@
         <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D15" t="s">
         <v>58</v>
@@ -1370,7 +1370,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J15" t="s">
         <v>69</v>
@@ -1379,27 +1379,27 @@
         <v>57</v>
       </c>
       <c r="L15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M15" t="s">
         <v>65</v>
       </c>
       <c r="N15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E16" t="s">
         <v>59</v>
@@ -1414,22 +1414,22 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K16" t="s">
         <v>60</v>
       </c>
       <c r="L16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M16" t="s">
         <v>23</v>
       </c>
       <c r="N16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
@@ -1440,7 +1440,7 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="D17" t="s">
         <v>66</v>
@@ -1458,7 +1458,7 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J17" t="s">
         <v>62</v>
@@ -1467,13 +1467,13 @@
         <v>63</v>
       </c>
       <c r="L17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M17" t="s">
         <v>64</v>
       </c>
       <c r="N17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
@@ -1484,7 +1484,7 @@
         <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D18" t="s">
         <v>58</v>
@@ -1502,7 +1502,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J18" t="s">
         <v>69</v>
@@ -1511,13 +1511,13 @@
         <v>70</v>
       </c>
       <c r="L18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M18" t="s">
         <v>71</v>
       </c>
       <c r="N18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
@@ -1528,7 +1528,7 @@
         <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D19" t="s">
         <v>72</v>
@@ -1546,22 +1546,22 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K19" t="s">
         <v>74</v>
       </c>
       <c r="L19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M19" t="s">
         <v>23</v>
       </c>
       <c r="N19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
@@ -1572,7 +1572,7 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="D20" t="s">
         <v>78</v>
@@ -1590,7 +1590,7 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J20" t="s">
         <v>53</v>
@@ -1599,13 +1599,13 @@
         <v>76</v>
       </c>
       <c r="L20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M20" t="s">
         <v>75</v>
       </c>
       <c r="N20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update user input script
</commit_message>
<xml_diff>
--- a/Models_Information.xlsx
+++ b/Models_Information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\tinyml-research-symposium-2022-haoyu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233A5FFE-5761-4747-94C7-07E633DEAE75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762B0BC4-FD7F-495C-BF88-DAF75B3ED4AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14330" yWindow="3910" windowWidth="21380" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -291,9 +291,6 @@
     <t>a sliding window of length 128 on 3d accelerometer data</t>
   </si>
   <si>
-    <t>https://github.com/Haoyu-R/TinyML-Research-Symposium-2022</t>
-  </si>
-  <si>
     <t>a NN for speech commands recognition left/right</t>
   </si>
   <si>
@@ -430,6 +427,9 @@
   </si>
   <si>
     <t>0: _silence_, 1: _unknown_,2: yes, 3: no, 4: up, 5: down, 6: left, 7: right, 8: on, 9: off, 10: stop, 11: go</t>
+  </si>
+  <si>
+    <t>https://experiments.withgoogle.com/tiny-motion-trainer</t>
   </si>
 </sst>
 </file>
@@ -777,7 +777,7 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -803,7 +803,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -815,13 +815,13 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
@@ -842,12 +842,12 @@
         <v>10</v>
       </c>
       <c r="O1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -856,10 +856,10 @@
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -871,30 +871,30 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J2" t="s">
         <v>50</v>
       </c>
       <c r="K2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -903,10 +903,10 @@
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -918,30 +918,30 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J3" t="s">
         <v>50</v>
       </c>
       <c r="K3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -950,10 +950,10 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E4" t="s">
         <v>114</v>
-      </c>
-      <c r="E4" t="s">
-        <v>115</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -965,30 +965,30 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -997,7 +997,7 @@
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E5" t="s">
         <v>56</v>
@@ -1012,25 +1012,25 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M5" t="s">
+        <v>117</v>
+      </c>
+      <c r="N5" t="s">
         <v>118</v>
       </c>
-      <c r="N5" t="s">
-        <v>119</v>
-      </c>
       <c r="O5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
@@ -1041,7 +1041,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D6" t="s">
         <v>82</v>
@@ -1059,25 +1059,25 @@
         <v>3</v>
       </c>
       <c r="I6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K6" t="s">
         <v>13</v>
       </c>
       <c r="L6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="O6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
@@ -1106,25 +1106,25 @@
         <v>4</v>
       </c>
       <c r="I7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K7" t="s">
         <v>19</v>
       </c>
       <c r="L7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M7" t="s">
         <v>20</v>
       </c>
       <c r="N7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
@@ -1135,13 +1135,13 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D8" t="s">
         <v>83</v>
       </c>
       <c r="E8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1153,7 +1153,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J8" t="s">
         <v>29</v>
@@ -1162,16 +1162,16 @@
         <v>30</v>
       </c>
       <c r="L8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M8" t="s">
         <v>20</v>
       </c>
       <c r="N8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
@@ -1182,7 +1182,7 @@
         <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D9" t="s">
         <v>39</v>
@@ -1200,7 +1200,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J9" t="s">
         <v>36</v>
@@ -1209,16 +1209,16 @@
         <v>37</v>
       </c>
       <c r="L9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M9" t="s">
         <v>32</v>
       </c>
       <c r="N9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
@@ -1229,7 +1229,7 @@
         <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D10" t="s">
         <v>52</v>
@@ -1247,25 +1247,25 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K10" t="s">
         <v>38</v>
       </c>
       <c r="L10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M10" t="s">
         <v>41</v>
       </c>
       <c r="N10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
@@ -1276,7 +1276,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D11" t="s">
         <v>64</v>
@@ -1294,7 +1294,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J11" t="s">
         <v>50</v>
@@ -1303,16 +1303,16 @@
         <v>15</v>
       </c>
       <c r="L11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M11" t="s">
         <v>14</v>
       </c>
       <c r="N11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
@@ -1323,7 +1323,7 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D12" t="s">
         <v>64</v>
@@ -1341,7 +1341,7 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J12" t="s">
         <v>50</v>
@@ -1350,16 +1350,16 @@
         <v>42</v>
       </c>
       <c r="L12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M12" t="s">
         <v>32</v>
       </c>
       <c r="N12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
@@ -1370,7 +1370,7 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D13" t="s">
         <v>64</v>
@@ -1388,7 +1388,7 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J13" t="s">
         <v>50</v>
@@ -1397,16 +1397,16 @@
         <v>43</v>
       </c>
       <c r="L13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M13" t="s">
         <v>20</v>
       </c>
       <c r="N13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
@@ -1417,7 +1417,7 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D14" t="s">
         <v>64</v>
@@ -1435,7 +1435,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J14" t="s">
         <v>50</v>
@@ -1444,16 +1444,16 @@
         <v>43</v>
       </c>
       <c r="L14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
@@ -1464,7 +1464,7 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D15" t="s">
         <v>64</v>
@@ -1482,7 +1482,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J15" t="s">
         <v>50</v>
@@ -1491,16 +1491,16 @@
         <v>43</v>
       </c>
       <c r="L15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
@@ -1511,7 +1511,7 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D16" t="s">
         <v>64</v>
@@ -1529,7 +1529,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J16" t="s">
         <v>50</v>
@@ -1538,16 +1538,16 @@
         <v>43</v>
       </c>
       <c r="L16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.35">
@@ -1558,7 +1558,7 @@
         <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D17" t="s">
         <v>78</v>
@@ -1576,25 +1576,25 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J17" t="s">
         <v>66</v>
       </c>
       <c r="K17" t="s">
-        <v>84</v>
+        <v>130</v>
       </c>
       <c r="L17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.35">
@@ -1605,7 +1605,7 @@
         <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D18" t="s">
         <v>78</v>
@@ -1623,25 +1623,25 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J18" t="s">
         <v>66</v>
       </c>
       <c r="K18" t="s">
-        <v>84</v>
+        <v>130</v>
       </c>
       <c r="L18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.35">
@@ -1652,7 +1652,7 @@
         <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D19" t="s">
         <v>55</v>
@@ -1670,7 +1670,7 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J19" t="s">
         <v>66</v>
@@ -1679,21 +1679,21 @@
         <v>54</v>
       </c>
       <c r="L19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M19" t="s">
         <v>62</v>
       </c>
       <c r="N19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -1702,7 +1702,7 @@
         <v>81</v>
       </c>
       <c r="D20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E20" t="s">
         <v>56</v>
@@ -1717,25 +1717,25 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K20" t="s">
         <v>57</v>
       </c>
       <c r="L20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M20" t="s">
         <v>20</v>
       </c>
       <c r="N20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.35">
@@ -1746,7 +1746,7 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D21" t="s">
         <v>63</v>
@@ -1764,7 +1764,7 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J21" t="s">
         <v>59</v>
@@ -1773,16 +1773,16 @@
         <v>60</v>
       </c>
       <c r="L21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M21" t="s">
         <v>61</v>
       </c>
       <c r="N21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="O21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.35">
@@ -1793,7 +1793,7 @@
         <v>31</v>
       </c>
       <c r="C22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D22" t="s">
         <v>55</v>
@@ -1811,7 +1811,7 @@
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J22" t="s">
         <v>66</v>
@@ -1820,16 +1820,16 @@
         <v>67</v>
       </c>
       <c r="L22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M22" t="s">
         <v>68</v>
       </c>
       <c r="N22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.35">
@@ -1858,25 +1858,25 @@
         <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K23" t="s">
         <v>71</v>
       </c>
       <c r="L23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M23" t="s">
         <v>20</v>
       </c>
       <c r="N23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.35">
@@ -1887,7 +1887,7 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D24" t="s">
         <v>75</v>
@@ -1905,7 +1905,7 @@
         <v>0</v>
       </c>
       <c r="I24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J24" t="s">
         <v>50</v>
@@ -1914,16 +1914,16 @@
         <v>73</v>
       </c>
       <c r="L24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M24" t="s">
         <v>72</v>
       </c>
       <c r="N24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>